<commit_message>
Files from the last run decided, the one without PELAGO age composition in 2023
</commit_message>
<xml_diff>
--- a/results/fleet_info.xlsx
+++ b/results/fleet_info.xlsx
@@ -460,13 +460,13 @@
         </is>
       </c>
       <c r="E4">
-        <v>2942295.490557186</v>
+        <v>4010862.399428019</v>
       </c>
       <c r="F4">
-        <v>5378286.662959828</v>
+        <v>5514711.46454878</v>
       </c>
       <c r="G4">
-        <v>1.827922001790968</v>
+        <v>1.374944068222141</v>
       </c>
     </row>
     <row r="5">
@@ -535,13 +535,13 @@
         </is>
       </c>
       <c r="E7">
-        <v>4877579.839276494</v>
+        <v>4716062.791582305</v>
       </c>
       <c r="F7">
-        <v>9304975.688940991</v>
+        <v>10139984.27183463</v>
       </c>
       <c r="G7">
-        <v>1.907703409386165</v>
+        <v>2.150095263772458</v>
       </c>
     </row>
     <row r="8">
@@ -610,13 +610,13 @@
         </is>
       </c>
       <c r="E10">
-        <v>1712922.494471447</v>
+        <v>1753540.568485639</v>
       </c>
       <c r="F10">
-        <v>7039447.840633143</v>
+        <v>7577626.45656653</v>
       </c>
       <c r="G10">
-        <v>4.10961258513059</v>
+        <v>4.321329425021847</v>
       </c>
     </row>
     <row r="11">
@@ -685,13 +685,13 @@
         </is>
       </c>
       <c r="E13">
-        <v>1310232.188112363</v>
+        <v>1781550.52851494</v>
       </c>
       <c r="F13">
-        <v>3214495.426357267</v>
+        <v>3463900.549746298</v>
       </c>
       <c r="G13">
-        <v>2.453378458812217</v>
+        <v>1.944317881701467</v>
       </c>
     </row>
     <row r="14">
@@ -760,13 +760,13 @@
         </is>
       </c>
       <c r="E16">
-        <v>1556458.657580097</v>
+        <v>2473879.59225941</v>
       </c>
       <c r="F16">
-        <v>1926211.661552823</v>
+        <v>2214201.27965111</v>
       </c>
       <c r="G16">
-        <v>1.237560440280245</v>
+        <v>0.8950319516678116</v>
       </c>
     </row>
     <row r="17">
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="E19">
-        <v>853619.4910017966</v>
+        <v>1150480.297765851</v>
       </c>
       <c r="F19">
-        <v>3362767.657418691</v>
+        <v>3879972.484502088</v>
       </c>
       <c r="G19">
-        <v>3.939422298654628</v>
+        <v>3.372480599656259</v>
       </c>
     </row>
     <row r="20">
@@ -910,13 +910,13 @@
         </is>
       </c>
       <c r="E22">
-        <v>3536262.936731075</v>
+        <v>4882664.9922407</v>
       </c>
       <c r="F22">
-        <v>631079.569303469</v>
+        <v>699714.482991705</v>
       </c>
       <c r="G22">
-        <v>0.1784594586416245</v>
+        <v>0.1433058553277069</v>
       </c>
     </row>
     <row r="23">
@@ -985,13 +985,13 @@
         </is>
       </c>
       <c r="E25">
-        <v>7423658.656196608</v>
+        <v>8902488.385420857</v>
       </c>
       <c r="F25">
-        <v>6268403.82751221</v>
+        <v>7274702.70611379</v>
       </c>
       <c r="G25">
-        <v>0.8443820113253598</v>
+        <v>0.8171538553228772</v>
       </c>
     </row>
     <row r="26">
@@ -1060,13 +1060,13 @@
         </is>
       </c>
       <c r="E28">
-        <v>5703983.728270975</v>
+        <v>8164487.498495134</v>
       </c>
       <c r="F28">
-        <v>6234793.853004176</v>
+        <v>6888111.95727473</v>
       </c>
       <c r="G28">
-        <v>1.093059543999454</v>
+        <v>0.8436674020928242</v>
       </c>
     </row>
     <row r="29">
@@ -1114,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>1.000000004273649</v>
+        <v>1.00000000230423</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1140,13 +1140,13 @@
         </is>
       </c>
       <c r="E31">
-        <v>6186247.627508745</v>
+        <v>7688747.31821244</v>
       </c>
       <c r="F31">
-        <v>14211027.11967381</v>
+        <v>15904284.1187412</v>
       </c>
       <c r="G31">
-        <v>2.297196616650263</v>
+        <v>2.068514344471759</v>
       </c>
     </row>
     <row r="32">
@@ -1215,13 +1215,13 @@
         </is>
       </c>
       <c r="E34">
-        <v>1690066.940434533</v>
+        <v>2348039.472705271</v>
       </c>
       <c r="F34">
-        <v>6130230.620613299</v>
+        <v>6562806.56005856</v>
       </c>
       <c r="G34">
-        <v>3.627211723955239</v>
+        <v>2.795015431532454</v>
       </c>
     </row>
     <row r="35">
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0.9999999925854568</v>
+        <v>1.00000000046291</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1295,13 +1295,13 @@
         </is>
       </c>
       <c r="E37">
-        <v>1836626.074427084</v>
+        <v>3210329.247209993</v>
       </c>
       <c r="F37">
-        <v>3198846.221202283</v>
+        <v>3529361.50628348</v>
       </c>
       <c r="G37">
-        <v>1.741697052950819</v>
+        <v>1.099376803594444</v>
       </c>
     </row>
     <row r="38">
@@ -1349,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>1.000000003953821</v>
+        <v>1.00000000086435</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1375,13 +1375,13 @@
         </is>
       </c>
       <c r="E40">
-        <v>2722302.10228866</v>
+        <v>5352586.981190261</v>
       </c>
       <c r="F40">
-        <v>7924417.418485777</v>
+        <v>9001634.912070677</v>
       </c>
       <c r="G40">
-        <v>2.910925062954497</v>
+        <v>1.681735382106574</v>
       </c>
     </row>
     <row r="41">
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0.9999999904938477</v>
+        <v>0.99999999750428</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1455,13 +1455,13 @@
         </is>
       </c>
       <c r="E43">
-        <v>3422952.815152428</v>
+        <v>5195648.527507986</v>
       </c>
       <c r="F43">
-        <v>8692950.668692511</v>
+        <v>9631787.113182543</v>
       </c>
       <c r="G43">
-        <v>2.539605755069517</v>
+        <v>1.853818067597864</v>
       </c>
     </row>
     <row r="44">
@@ -1530,13 +1530,13 @@
         </is>
       </c>
       <c r="E46">
-        <v>1180260.437170755</v>
+        <v>2261217.178708012</v>
       </c>
       <c r="F46">
-        <v>4988959.284160127</v>
+        <v>5607539.553918083</v>
       </c>
       <c r="G46">
-        <v>4.226998658126117</v>
+        <v>2.479876593331939</v>
       </c>
     </row>
     <row r="47">
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0.9999999923873726</v>
+        <v>1.000000001788306</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1610,13 +1610,13 @@
         </is>
       </c>
       <c r="E49">
-        <v>781315.6657888193</v>
+        <v>1522802.581186213</v>
       </c>
       <c r="F49">
-        <v>5393324.43815508</v>
+        <v>5861286.777441995</v>
       </c>
       <c r="G49">
-        <v>6.902875078934913</v>
+        <v>3.849012898885583</v>
       </c>
     </row>
     <row r="50">
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>0.9999999961759474</v>
+        <v>1.00000000315792</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -1690,13 +1690,13 @@
         </is>
       </c>
       <c r="E52">
-        <v>1384905.75918492</v>
+        <v>1394047.989490662</v>
       </c>
       <c r="F52">
-        <v>5432468.634291687</v>
+        <v>5788172.932016804</v>
       </c>
       <c r="G52">
-        <v>3.922626935632747</v>
+        <v>4.152061461048847</v>
       </c>
     </row>
     <row r="53">
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>0.99999999697907</v>
+        <v>1.000000007574021</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>1.000000005905129</v>
+        <v>1.000000000595972</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -1775,13 +1775,13 @@
         </is>
       </c>
       <c r="E55">
-        <v>1644344.54929226</v>
+        <v>1998547.884679702</v>
       </c>
       <c r="F55">
-        <v>5118893.620107203</v>
+        <v>5228907.70030661</v>
       </c>
       <c r="G55">
-        <v>3.113029822314562</v>
+        <v>2.616353473634495</v>
       </c>
     </row>
     <row r="56">
@@ -1802,13 +1802,13 @@
         </is>
       </c>
       <c r="E56">
-        <v>2826382.966222246</v>
+        <v>2250982.808710504</v>
       </c>
       <c r="F56">
-        <v>0.9999999978499117</v>
+        <v>0.9999999909726178</v>
       </c>
       <c r="G56">
-        <v>3.538090944506772e-07</v>
+        <v>4.442503901420184e-07</v>
       </c>
     </row>
     <row r="57">
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0.9999999972182998</v>
+        <v>1.000000003737489</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -1858,13 +1858,13 @@
         </is>
       </c>
       <c r="E58">
-        <v>3479679.668903098</v>
+        <v>3778678.969770925</v>
       </c>
       <c r="F58">
-        <v>6657845.04554708</v>
+        <v>7185863.828460072</v>
       </c>
       <c r="G58">
-        <v>1.913349985932998</v>
+        <v>1.90168677623749</v>
       </c>
     </row>
     <row r="59">
@@ -1912,7 +1912,7 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <v>0.9999999959938732</v>
+        <v>0.9999999984275501</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -1938,13 +1938,13 @@
         </is>
       </c>
       <c r="E61">
-        <v>6032964.371716144</v>
+        <v>3927210.251292792</v>
       </c>
       <c r="F61">
-        <v>2491055.610547951</v>
+        <v>2812404.857870263</v>
       </c>
       <c r="G61">
-        <v>0.4129073962754636</v>
+        <v>0.7161329997405796</v>
       </c>
     </row>
     <row r="62">
@@ -1965,13 +1965,13 @@
         </is>
       </c>
       <c r="E62">
-        <v>988999.2391163338</v>
+        <v>553314.5940991236</v>
       </c>
       <c r="F62">
-        <v>0.999999993384184</v>
+        <v>1.000000001949737</v>
       </c>
       <c r="G62">
-        <v>1.011123117018451e-06</v>
+        <v>1.807290125028931e-06</v>
       </c>
     </row>
     <row r="63">
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>1.000000002363022</v>
+        <v>0.9999999987871</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2021,13 +2021,13 @@
         </is>
       </c>
       <c r="E64">
-        <v>1076307.287067227</v>
+        <v>819552.945456011</v>
       </c>
       <c r="F64">
-        <v>2464268.30704905</v>
+        <v>2721637.306061814</v>
       </c>
       <c r="G64">
-        <v>2.289558322850164</v>
+        <v>3.320880391135018</v>
       </c>
     </row>
     <row r="65">
@@ -2048,13 +2048,13 @@
         </is>
       </c>
       <c r="E65">
-        <v>839610.7641502484</v>
+        <v>560991.1729625323</v>
       </c>
       <c r="F65">
-        <v>0.9999999949027396</v>
+        <v>1.000000000646086</v>
       </c>
       <c r="G65">
-        <v>1.191028078248637e-06</v>
+        <v>1.782559243071859e-06</v>
       </c>
     </row>
     <row r="66">
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>1.000000000303378</v>
+        <v>1.00000000785463</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2104,13 +2104,13 @@
         </is>
       </c>
       <c r="E67">
-        <v>620640.2072074591</v>
+        <v>846565.0261066078</v>
       </c>
       <c r="F67">
-        <v>2658288.264772855</v>
+        <v>2656680.238955629</v>
       </c>
       <c r="G67">
-        <v>4.28313898117187</v>
+        <v>3.138188038754478</v>
       </c>
     </row>
     <row r="68">
@@ -2179,13 +2179,13 @@
         </is>
       </c>
       <c r="E70">
-        <v>5295487.557734448</v>
+        <v>8330208.101267722</v>
       </c>
       <c r="F70">
-        <v>6521270.24868184</v>
+        <v>7002590.642403614</v>
       </c>
       <c r="G70">
-        <v>1.231476833357307</v>
+        <v>0.8406261352988208</v>
       </c>
     </row>
     <row r="71">
@@ -2254,13 +2254,13 @@
         </is>
       </c>
       <c r="E73">
-        <v>3647762.117733285</v>
+        <v>2170667.656335704</v>
       </c>
       <c r="F73">
-        <v>3961254.596482811</v>
+        <v>4508156.510163746</v>
       </c>
       <c r="G73">
-        <v>1.085941042379247</v>
+        <v>2.076852482233023</v>
       </c>
     </row>
     <row r="74">
@@ -2281,13 +2281,13 @@
         </is>
       </c>
       <c r="E74">
-        <v>1931508.227289685</v>
+        <v>2030548.155792167</v>
       </c>
       <c r="F74">
-        <v>1.000000006933837</v>
+        <v>0.9999999857464693</v>
       </c>
       <c r="G74">
-        <v>5.177301306849978e-07</v>
+        <v>4.924778478628814e-07</v>
       </c>
     </row>
     <row r="75">
@@ -2311,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>0.9999999963931374</v>
+        <v>0.999999999848072</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2337,13 +2337,13 @@
         </is>
       </c>
       <c r="E76">
-        <v>2258762.999905685</v>
+        <v>3135815.849344484</v>
       </c>
       <c r="F76">
-        <v>5257190.205955083</v>
+        <v>5879944.736744782</v>
       </c>
       <c r="G76">
-        <v>2.327464282961336</v>
+        <v>1.875092486050778</v>
       </c>
     </row>
     <row r="77">
@@ -2364,13 +2364,13 @@
         </is>
       </c>
       <c r="E77">
-        <v>1809408.841099476</v>
+        <v>1507755.091040642</v>
       </c>
       <c r="F77">
-        <v>0.9999999920032994</v>
+        <v>1.000000002839909</v>
       </c>
       <c r="G77">
-        <v>5.526666883066933e-07</v>
+        <v>6.63237689451087e-07</v>
       </c>
     </row>
     <row r="78">
@@ -2394,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="F78">
-        <v>0.9999999965620188</v>
+        <v>0.999999999158762</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2420,13 +2420,13 @@
         </is>
       </c>
       <c r="E79">
-        <v>1237709.764288835</v>
+        <v>2478304.637381603</v>
       </c>
       <c r="F79">
-        <v>9113804.446800129</v>
+        <v>9654530.838541202</v>
       </c>
       <c r="G79">
-        <v>7.363442310755909</v>
+        <v>3.895619082866859</v>
       </c>
     </row>
     <row r="80">
@@ -2447,13 +2447,13 @@
         </is>
       </c>
       <c r="E80">
-        <v>1160817.316443804</v>
+        <v>903285.0225595324</v>
       </c>
       <c r="F80">
-        <v>1.000000002375354</v>
+        <v>0.999999996095956</v>
       </c>
       <c r="G80">
-        <v>8.614619959658098e-07</v>
+        <v>1.107070272528569e-06</v>
       </c>
     </row>
     <row r="81">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="F81">
-        <v>1.000000004804592</v>
+        <v>0.9999999891340161</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -2503,13 +2503,13 @@
         </is>
       </c>
       <c r="E82">
-        <v>859696.8593422457</v>
+        <v>1503754.108973784</v>
       </c>
       <c r="F82">
-        <v>6521238.107010044</v>
+        <v>6568082.336603807</v>
       </c>
       <c r="G82">
-        <v>7.585508817607459</v>
+        <v>4.367790117684933</v>
       </c>
     </row>
     <row r="83">
@@ -2530,13 +2530,13 @@
         </is>
       </c>
       <c r="E83">
-        <v>1497771.37699823</v>
+        <v>1152889.052376504</v>
       </c>
       <c r="F83">
-        <v>0.9999999892264257</v>
+        <v>1.000000008176831</v>
       </c>
       <c r="G83">
-        <v>6.676586324079601e-07</v>
+        <v>8.673861601127051e-07</v>
       </c>
     </row>
     <row r="84">
@@ -2560,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <v>0.9999999914065589</v>
+        <v>0.9999999982906704</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -2586,13 +2586,13 @@
         </is>
       </c>
       <c r="E85">
-        <v>1794157.380376586</v>
+        <v>2122141.497247829</v>
       </c>
       <c r="F85">
-        <v>5707525.979746813</v>
+        <v>5760693.69800827</v>
       </c>
       <c r="G85">
-        <v>3.181173537044353</v>
+        <v>2.714566255586266</v>
       </c>
     </row>
     <row r="86">
@@ -2613,13 +2613,13 @@
         </is>
       </c>
       <c r="E86">
-        <v>871473.974891482</v>
+        <v>670779.4992317396</v>
       </c>
       <c r="F86">
-        <v>1.000000013085012</v>
+        <v>0.999999989396481</v>
       </c>
       <c r="G86">
-        <v>1.14748121217221e-06</v>
+        <v>1.490802850328321e-06</v>
       </c>
     </row>
     <row r="87">
@@ -2643,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <v>1.000000000360383</v>
+        <v>0.999999996748363</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -2669,13 +2669,13 @@
         </is>
       </c>
       <c r="E88">
-        <v>696350.828750234</v>
+        <v>971629.0153496976</v>
       </c>
       <c r="F88">
-        <v>5180084.129582084</v>
+        <v>5228583.512319434</v>
       </c>
       <c r="G88">
-        <v>7.438899927611156</v>
+        <v>5.381255015771242</v>
       </c>
     </row>
     <row r="89">
@@ -2696,13 +2696,13 @@
         </is>
       </c>
       <c r="E89">
-        <v>838107.5699975909</v>
+        <v>424657.5954804751</v>
       </c>
       <c r="F89">
-        <v>0.9999999996410421</v>
+        <v>1.00000000562151</v>
       </c>
       <c r="G89">
-        <v>1.193164261293949e-06</v>
+        <v>2.354838383356994e-06</v>
       </c>
     </row>
     <row r="90">
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <v>1.000000006594427</v>
+        <v>1.000000000821403</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -2752,13 +2752,13 @@
         </is>
       </c>
       <c r="E91">
-        <v>596879.9290381279</v>
+        <v>614933.5397632965</v>
       </c>
       <c r="F91">
-        <v>3681053.860628297</v>
+        <v>3784340.429751332</v>
       </c>
       <c r="G91">
-        <v>6.167159727686465</v>
+        <v>6.154064114323672</v>
       </c>
     </row>
     <row r="92">
@@ -2779,13 +2779,13 @@
         </is>
       </c>
       <c r="E92">
-        <v>2585317.89158569</v>
+        <v>1707092.310604753</v>
       </c>
       <c r="F92">
-        <v>1.000000002003415</v>
+        <v>1.000000003666415</v>
       </c>
       <c r="G92">
-        <v>3.867996292672816e-07</v>
+        <v>5.857914053354011e-07</v>
       </c>
     </row>
     <row r="93">
@@ -2809,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="F93">
-        <v>1.000000000898834</v>
+        <v>1.000000007280829</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -2835,13 +2835,13 @@
         </is>
       </c>
       <c r="E94">
-        <v>3309002.03858812</v>
+        <v>3206574.582082749</v>
       </c>
       <c r="F94">
-        <v>4617635.502905988</v>
+        <v>4639679.870985954</v>
       </c>
       <c r="G94">
-        <v>1.395476777909824</v>
+        <v>1.446927165490212</v>
       </c>
     </row>
     <row r="95">
@@ -2862,13 +2862,13 @@
         </is>
       </c>
       <c r="E95">
-        <v>2965081.496701077</v>
+        <v>2322890.264100066</v>
       </c>
       <c r="F95">
-        <v>1.000000002931492</v>
+        <v>1.000000002877993</v>
       </c>
       <c r="G95">
-        <v>3.372588591727017e-07</v>
+        <v>4.304981678785471e-07</v>
       </c>
     </row>
     <row r="96">
@@ -2892,7 +2892,7 @@
         <v>0</v>
       </c>
       <c r="F96">
-        <v>1.00000001113397</v>
+        <v>1.000000000415156</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -2918,13 +2918,13 @@
         </is>
       </c>
       <c r="E97">
-        <v>3465591.194447174</v>
+        <v>3936005.376361746</v>
       </c>
       <c r="F97">
-        <v>6316470.668895728</v>
+        <v>6657550.13409682</v>
       </c>
       <c r="G97">
-        <v>1.822624283849879</v>
+        <v>1.691448435024939</v>
       </c>
     </row>
     <row r="98">
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="F99">
-        <v>1.00000000036504</v>
+        <v>0.99999999764986</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -2998,13 +2998,13 @@
         </is>
       </c>
       <c r="E100">
-        <v>1286379.479684115</v>
+        <v>2958551.508941003</v>
       </c>
       <c r="F100">
-        <v>6332735.267905084</v>
+        <v>6589268.456718239</v>
       </c>
       <c r="G100">
-        <v>4.922913780823183</v>
+        <v>2.227194097113026</v>
       </c>
     </row>
     <row r="101">
@@ -3052,7 +3052,7 @@
         <v>0</v>
       </c>
       <c r="F102">
-        <v>0.9999999918151925</v>
+        <v>0.9999999946932759</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -3078,13 +3078,13 @@
         </is>
       </c>
       <c r="E103">
-        <v>2727504.517121038</v>
+        <v>1681441.921393492</v>
       </c>
       <c r="F103">
-        <v>5276626.0456231</v>
+        <v>5308865.722438828</v>
       </c>
       <c r="G103">
-        <v>1.934598462624265</v>
+        <v>3.157329227309329</v>
       </c>
     </row>
     <row r="104">
@@ -3132,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="F105">
-        <v>1.000000013231183</v>
+        <v>1.000000005134101</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -3158,13 +3158,13 @@
         </is>
       </c>
       <c r="E106">
-        <v>419524.740371756</v>
+        <v>2447821.588502292</v>
       </c>
       <c r="F106">
-        <v>2917173.553453564</v>
+        <v>3367307.353078973</v>
       </c>
       <c r="G106">
-        <v>6.953519715830232</v>
+        <v>1.375634306395374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>